<commit_message>
Reminder: before changing table 3
</commit_message>
<xml_diff>
--- a/working/Perturb/log/tables/table1.xlsx
+++ b/working/Perturb/log/tables/table1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab_codes\FEM\FiniteElemntMethod\working\Perturb\log\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122C64EA-669B-4C32-A37C-B10F539CBB91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDC8C69-3669-49A4-A159-13B0FF0B64EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="1800" windowWidth="16440" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="-108" windowWidth="22128" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>L2</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>$10^{-5}$</t>
+  </si>
+  <si>
+    <t>$2^{-8}$</t>
   </si>
 </sst>
 </file>
@@ -89,7 +92,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -144,13 +147,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -159,7 +162,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -168,6 +171,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -450,19 +456,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ19"/>
+  <dimension ref="A1:AW19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>0</v>
       </c>
@@ -485,636 +492,726 @@
         <v>6</v>
       </c>
       <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
         <v>0</v>
       </c>
-      <c r="J1">
+      <c r="K1">
         <v>1</v>
       </c>
-      <c r="K1">
+      <c r="L1">
         <v>2</v>
       </c>
-      <c r="L1">
+      <c r="M1">
         <v>3</v>
       </c>
-      <c r="M1">
+      <c r="N1">
         <v>4</v>
       </c>
-      <c r="N1">
+      <c r="O1">
         <v>5</v>
       </c>
-      <c r="O1">
+      <c r="P1">
         <v>6</v>
       </c>
-      <c r="P1">
+      <c r="Q1">
+        <v>7</v>
+      </c>
+      <c r="R1">
         <v>0</v>
       </c>
-      <c r="Q1">
+      <c r="S1">
         <v>1</v>
       </c>
-      <c r="R1">
+      <c r="T1">
         <v>2</v>
       </c>
-      <c r="S1">
+      <c r="U1">
         <v>3</v>
       </c>
-      <c r="T1">
+      <c r="V1">
         <v>4</v>
       </c>
-      <c r="U1">
+      <c r="W1">
         <v>5</v>
       </c>
-      <c r="V1">
+      <c r="X1">
         <v>6</v>
       </c>
-      <c r="W1">
+      <c r="Y1">
+        <v>7</v>
+      </c>
+      <c r="Z1">
         <v>0</v>
       </c>
-      <c r="X1">
+      <c r="AA1">
         <v>1</v>
       </c>
-      <c r="Y1">
+      <c r="AB1">
         <v>2</v>
       </c>
-      <c r="Z1">
+      <c r="AC1">
         <v>3</v>
       </c>
-      <c r="AA1">
+      <c r="AD1">
         <v>4</v>
       </c>
-      <c r="AB1">
+      <c r="AE1">
         <v>5</v>
       </c>
-      <c r="AC1">
+      <c r="AF1">
         <v>6</v>
       </c>
-      <c r="AD1">
+      <c r="AG1">
+        <v>7</v>
+      </c>
+      <c r="AH1">
         <v>0</v>
       </c>
-      <c r="AE1">
+      <c r="AI1">
         <v>1</v>
       </c>
-      <c r="AF1">
+      <c r="AJ1">
         <v>2</v>
       </c>
-      <c r="AG1">
+      <c r="AK1">
         <v>3</v>
       </c>
-      <c r="AH1">
+      <c r="AL1">
         <v>4</v>
       </c>
-      <c r="AI1">
+      <c r="AM1">
         <v>5</v>
       </c>
-      <c r="AJ1">
+      <c r="AN1">
         <v>6</v>
       </c>
-      <c r="AK1">
+      <c r="AO1">
+        <v>7</v>
+      </c>
+      <c r="AP1">
         <v>0</v>
       </c>
-      <c r="AL1">
+      <c r="AQ1">
         <v>1</v>
       </c>
-      <c r="AM1">
+      <c r="AR1">
         <v>2</v>
       </c>
-      <c r="AN1">
+      <c r="AS1">
         <v>3</v>
       </c>
-      <c r="AO1">
+      <c r="AT1">
         <v>4</v>
       </c>
-      <c r="AP1">
+      <c r="AU1">
         <v>5</v>
       </c>
-      <c r="AQ1">
+      <c r="AV1">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="AW1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.147784664075199</v>
+        <v>0.14613029776269401</v>
       </c>
       <c r="C2">
-        <v>4.1304988971907097E-2</v>
+        <v>4.11748279722223E-2</v>
       </c>
       <c r="D2">
-        <v>9.0541893006924508E-3</v>
+        <v>9.0373839369018698E-3</v>
       </c>
       <c r="E2">
-        <v>2.02982222462833E-3</v>
+        <v>2.0284652947525298E-3</v>
       </c>
       <c r="F2">
-        <v>4.8592583523819101E-4</v>
+        <v>4.8583406358802502E-4</v>
       </c>
       <c r="G2">
-        <v>1.19960438652214E-4</v>
+        <v>1.1995457850497299E-4</v>
       </c>
       <c r="H2" s="1">
-        <v>2.9891800138791299E-5</v>
-      </c>
-      <c r="I2">
-        <v>0.137211458232564</v>
+        <v>2.9891430663796301E-5</v>
+      </c>
+      <c r="I2" s="1">
+        <v>7.4675517319404698E-6</v>
       </c>
       <c r="J2">
-        <v>5.2834283897587903E-2</v>
+        <v>0.13921311725056401</v>
       </c>
       <c r="K2">
-        <v>1.26610716471319E-2</v>
+        <v>5.2762560634564103E-2</v>
       </c>
       <c r="L2">
-        <v>3.0346332472407302E-3</v>
+        <v>1.26497474793534E-2</v>
       </c>
       <c r="M2">
-        <v>7.44095224979972E-4</v>
+        <v>3.0337373961639201E-3</v>
       </c>
       <c r="N2">
-        <v>1.8490617824211999E-4</v>
-      </c>
-      <c r="O2" s="1">
-        <v>4.6152388751748703E-5</v>
-      </c>
-      <c r="P2">
-        <v>0.157921667131632</v>
-      </c>
-      <c r="Q2">
-        <v>5.8759696541900303E-2</v>
+        <v>7.4403548136680795E-4</v>
+      </c>
+      <c r="O2">
+        <v>1.8490237644745399E-4</v>
+      </c>
+      <c r="P2" s="1">
+        <v>4.61521509594925E-5</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1.1533289358058799E-5</v>
       </c>
       <c r="R2">
-        <v>1.23073837055576E-2</v>
+        <v>0.16014807773763401</v>
       </c>
       <c r="S2">
-        <v>2.90844416658936E-3</v>
+        <v>5.8710949271866097E-2</v>
       </c>
       <c r="T2">
-        <v>8.5766845008287203E-4</v>
+        <v>1.22966162398111E-2</v>
       </c>
       <c r="U2">
-        <v>2.4258304728881199E-4</v>
-      </c>
-      <c r="V2" s="1">
-        <v>6.3214799570935498E-5</v>
+        <v>2.90752763836833E-3</v>
+      </c>
+      <c r="V2">
+        <v>8.5761684203924395E-4</v>
       </c>
       <c r="W2">
-        <v>0.158244390333554</v>
-      </c>
-      <c r="X2">
-        <v>5.8833861041802299E-2</v>
-      </c>
-      <c r="Y2">
-        <v>1.2013770619483799E-2</v>
+        <v>2.42580150319439E-4</v>
+      </c>
+      <c r="X2" s="1">
+        <v>6.3214620661913203E-5</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1.5978545303006598E-5</v>
       </c>
       <c r="Z2">
-        <v>2.4316436631936899E-3</v>
+        <v>0.16047095760150501</v>
       </c>
       <c r="AA2">
-        <v>5.5855883415755695E-4</v>
+        <v>5.8785514208246799E-2</v>
       </c>
       <c r="AB2">
-        <v>1.4177721582094699E-4</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>4.0218468844292803E-5</v>
+        <v>1.2002798593761599E-2</v>
+      </c>
+      <c r="AC2">
+        <v>2.4305515280036898E-3</v>
       </c>
       <c r="AD2">
-        <v>0.158247633203555</v>
+        <v>5.5847973967305899E-4</v>
       </c>
       <c r="AE2">
-        <v>5.8834611201709401E-2</v>
-      </c>
-      <c r="AF2">
-        <v>1.20106472564001E-2</v>
-      </c>
-      <c r="AG2">
-        <v>2.42515574654445E-3</v>
+        <v>1.4177226816617299E-4</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>4.0218201038490698E-5</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>1.26287167580191E-5</v>
       </c>
       <c r="AH2">
-        <v>5.5058977608645604E-4</v>
+        <v>0.16047420174990601</v>
       </c>
       <c r="AI2">
-        <v>1.33653178925359E-4</v>
-      </c>
-      <c r="AJ2" s="1">
-        <v>3.3212739885418801E-5</v>
+        <v>5.8786268424612903E-2</v>
+      </c>
+      <c r="AJ2">
+        <v>1.19996730213488E-2</v>
       </c>
       <c r="AK2">
-        <v>0.158247665633824</v>
+        <v>2.4240607498218101E-3</v>
       </c>
       <c r="AL2">
-        <v>5.88346187042285E-2</v>
+        <v>5.5050944312172098E-4</v>
       </c>
       <c r="AM2">
-        <v>1.2010616005437401E-2</v>
-      </c>
-      <c r="AN2">
-        <v>2.4250906631563302E-3</v>
-      </c>
-      <c r="AO2">
-        <v>5.5050893772737503E-4</v>
+        <v>1.33647928976621E-4</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>3.32123913606659E-5</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>8.3524501285831199E-6</v>
       </c>
       <c r="AP2">
-        <v>1.3356701960643601E-4</v>
-      </c>
-      <c r="AQ2" s="1">
-        <v>3.3125076068268897E-5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
+        <v>0.16047423419293</v>
+      </c>
+      <c r="AQ2">
+        <v>5.8786275967702001E-2</v>
+      </c>
+      <c r="AR2">
+        <v>1.19996417482776E-2</v>
+      </c>
+      <c r="AS2">
+        <v>2.4239956376513202E-3</v>
+      </c>
+      <c r="AT2">
+        <v>5.5042859315781404E-4</v>
+      </c>
+      <c r="AU2">
+        <v>1.3356176624171001E-4</v>
+      </c>
+      <c r="AV2" s="1">
+        <v>3.3124726935065003E-5</v>
+      </c>
+      <c r="AW2" s="1">
+        <v>8.2648880703265706E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.1391196006028901</v>
+        <v>1.1024819124702701</v>
       </c>
       <c r="C3">
-        <v>0.60166252581349</v>
+        <v>0.60207466105854701</v>
       </c>
       <c r="D3">
-        <v>0.17817582653227601</v>
+        <v>0.17819583915298301</v>
       </c>
       <c r="E3">
-        <v>4.6719581601742E-2</v>
+        <v>4.6720513065551902E-2</v>
       </c>
       <c r="F3">
-        <v>1.1821944233793E-2</v>
+        <v>1.1821994920903999E-2</v>
       </c>
       <c r="G3">
-        <v>2.9644258317228999E-3</v>
+        <v>2.9644288559223199E-3</v>
       </c>
       <c r="H3">
-        <v>7.4166664596875395E-4</v>
+        <v>7.4166681556407101E-4</v>
       </c>
       <c r="I3">
-        <v>1.23411430422914</v>
+        <v>1.85459648045657E-4</v>
       </c>
       <c r="J3">
-        <v>0.69199276042830504</v>
+        <v>1.2037206551459601</v>
       </c>
       <c r="K3">
-        <v>0.20437167990684199</v>
+        <v>0.69235088152040303</v>
       </c>
       <c r="L3">
-        <v>5.3537196606628798E-2</v>
+        <v>0.20439233350206101</v>
       </c>
       <c r="M3">
-        <v>1.3549233033131901E-2</v>
+        <v>5.3538319443851401E-2</v>
       </c>
       <c r="N3">
-        <v>3.3979215093523601E-3</v>
+        <v>1.35492993157037E-2</v>
       </c>
       <c r="O3">
-        <v>8.5014995534273799E-4</v>
+        <v>3.3979255775746001E-3</v>
       </c>
       <c r="P3">
-        <v>1.3310574844008201</v>
+        <v>8.5015028141182899E-4</v>
       </c>
       <c r="Q3">
-        <v>0.78193364657342801</v>
+        <v>2.1257895171689501E-4</v>
       </c>
       <c r="R3">
-        <v>0.24491634634602899</v>
+        <v>1.3019405588973101</v>
       </c>
       <c r="S3">
-        <v>6.3719480241545806E-2</v>
+        <v>0.78221070039045704</v>
       </c>
       <c r="T3">
-        <v>1.5584892985394E-2</v>
+        <v>0.244930874275224</v>
       </c>
       <c r="U3">
-        <v>3.84612438239175E-3</v>
+        <v>6.3720228446790997E-2</v>
       </c>
       <c r="V3">
-        <v>9.5986975572740895E-4</v>
+        <v>1.55849508893064E-2</v>
       </c>
       <c r="W3">
-        <v>1.3325178015756201</v>
+        <v>3.8461284978469198E-3</v>
       </c>
       <c r="X3">
-        <v>0.78450218865265198</v>
+        <v>9.5987022566530701E-4</v>
       </c>
       <c r="Y3">
-        <v>0.248998881823014</v>
+        <v>2.39973192928815E-4</v>
       </c>
       <c r="Z3">
-        <v>6.7134810805705894E-2</v>
+        <v>1.30341454825545</v>
       </c>
       <c r="AA3">
-        <v>1.7150157144569099E-2</v>
+        <v>0.78477685610941195</v>
       </c>
       <c r="AB3">
-        <v>4.2838657430498001E-3</v>
+        <v>0.249012599250546</v>
       </c>
       <c r="AC3">
-        <v>1.04549805776842E-3</v>
+        <v>6.7135277082926603E-2</v>
       </c>
       <c r="AD3">
-        <v>1.33253247602346</v>
+        <v>1.7150175080585299E-2</v>
       </c>
       <c r="AE3">
-        <v>0.784528477201616</v>
+        <v>4.2838668903312704E-3</v>
       </c>
       <c r="AF3">
-        <v>0.24904520690187701</v>
+        <v>1.0454984410289199E-3</v>
       </c>
       <c r="AG3">
-        <v>6.7189867089987296E-2</v>
+        <v>2.5031958796012502E-4</v>
       </c>
       <c r="AH3">
-        <v>1.7207159227806301E-2</v>
+        <v>1.3034293595205999</v>
       </c>
       <c r="AI3">
-        <v>4.33783794866125E-3</v>
+        <v>0.78480312028907495</v>
       </c>
       <c r="AJ3">
-        <v>1.08761027260846E-3</v>
+        <v>0.24905891540272301</v>
       </c>
       <c r="AK3">
-        <v>1.3325326227751</v>
+        <v>6.7190328925909107E-2</v>
       </c>
       <c r="AL3">
-        <v>0.784528740149119</v>
+        <v>1.7207176396937598E-2</v>
       </c>
       <c r="AM3">
-        <v>0.24904567078168499</v>
+        <v>4.3378386757803901E-3</v>
       </c>
       <c r="AN3">
-        <v>6.7190421029465805E-2</v>
+        <v>1.0876104864705901E-3</v>
       </c>
       <c r="AO3">
-        <v>1.7207743812933898E-2</v>
+        <v>2.7184376503633302E-4</v>
       </c>
       <c r="AP3">
-        <v>4.3384337795367104E-3</v>
+        <v>1.3034295076404201</v>
       </c>
       <c r="AQ3">
-        <v>1.08820927598601E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
+        <v>0.78480338299283303</v>
+      </c>
+      <c r="AR3">
+        <v>0.249059379193175</v>
+      </c>
+      <c r="AS3">
+        <v>6.7190882820731102E-2</v>
+      </c>
+      <c r="AT3">
+        <v>1.7207760964826901E-2</v>
+      </c>
+      <c r="AU3">
+        <v>4.33843450211334E-3</v>
+      </c>
+      <c r="AV3">
+        <v>1.0882094891914E-3</v>
+      </c>
+      <c r="AW3">
+        <v>2.7243758575696002E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>13.1213991232962</v>
+        <v>13.388951370614899</v>
       </c>
       <c r="C4">
-        <v>8.1654945384054205</v>
+        <v>8.1657151869805293</v>
       </c>
       <c r="D4">
-        <v>4.0133833119946098</v>
+        <v>4.0133887657064804</v>
       </c>
       <c r="E4">
-        <v>1.9423390864662899</v>
+        <v>1.9423393095046999</v>
       </c>
       <c r="F4">
-        <v>0.95509572822142896</v>
+        <v>0.955095754095312</v>
       </c>
       <c r="G4">
-        <v>0.47396478927392999</v>
+        <v>0.47396479151254201</v>
       </c>
       <c r="H4">
-        <v>0.23615991499941899</v>
+        <v>0.23615991515123899</v>
       </c>
       <c r="I4">
-        <v>13.072486564038501</v>
+        <v>0.117884264261119</v>
       </c>
       <c r="J4">
-        <v>8.6873798718995108</v>
+        <v>13.3744533285515</v>
       </c>
       <c r="K4">
-        <v>4.14900076611272</v>
+        <v>8.6875748200293597</v>
       </c>
       <c r="L4">
-        <v>1.96478966024571</v>
+        <v>4.1490101609472303</v>
       </c>
       <c r="M4">
-        <v>0.95880760520756803</v>
+        <v>1.9647901197689399</v>
       </c>
       <c r="N4">
-        <v>0.47464660775579398</v>
+        <v>0.95880764694293796</v>
       </c>
       <c r="O4">
-        <v>0.23629943835839801</v>
+        <v>0.47464661101879702</v>
       </c>
       <c r="P4">
-        <v>13.274197288571701</v>
+        <v>0.23629943869501899</v>
       </c>
       <c r="Q4">
-        <v>9.7639462684590193</v>
+        <v>0.117915263449834</v>
       </c>
       <c r="R4">
-        <v>5.3969574077597704</v>
+        <v>13.579187321393301</v>
       </c>
       <c r="S4">
-        <v>2.5351019531711398</v>
+        <v>9.7638008706783701</v>
       </c>
       <c r="T4">
-        <v>1.0851297588615001</v>
+        <v>5.3969560100312197</v>
       </c>
       <c r="U4">
-        <v>0.49130798920282998</v>
+        <v>2.53510224561394</v>
       </c>
       <c r="V4">
-        <v>0.23828989378837601</v>
+        <v>1.0851297958228601</v>
       </c>
       <c r="W4">
-        <v>13.2777802365939</v>
+        <v>0.49130799796350799</v>
       </c>
       <c r="X4">
-        <v>9.8035163842577493</v>
+        <v>0.23828989315422899</v>
       </c>
       <c r="Y4">
-        <v>5.5857868723259996</v>
+        <v>0.11816932418666699</v>
       </c>
       <c r="Z4">
-        <v>2.9089908616373101</v>
+        <v>13.582773732899</v>
       </c>
       <c r="AA4">
-        <v>1.46137630178766</v>
+        <v>9.8033577390748192</v>
       </c>
       <c r="AB4">
-        <v>0.71402283903758101</v>
+        <v>5.5857831363782697</v>
       </c>
       <c r="AC4">
-        <v>0.329213866204696</v>
+        <v>2.90899078599718</v>
       </c>
       <c r="AD4">
-        <v>13.277816333013</v>
+        <v>1.46137630713592</v>
       </c>
       <c r="AE4">
-        <v>9.8039231583150404</v>
+        <v>0.71402283664759303</v>
       </c>
       <c r="AF4">
-        <v>5.5879356536051104</v>
+        <v>0.32921387473970398</v>
       </c>
       <c r="AG4">
-        <v>2.9149193650583798</v>
+        <v>0.140716946989564</v>
       </c>
       <c r="AH4">
-        <v>1.4743269896648901</v>
+        <v>13.582809858350601</v>
       </c>
       <c r="AI4">
-        <v>0.73911912755119302</v>
+        <v>9.8037643774652299</v>
       </c>
       <c r="AJ4">
-        <v>0.36939568685580798</v>
+        <v>5.5879318912330502</v>
       </c>
       <c r="AK4">
-        <v>13.2778166940041</v>
+        <v>2.9149192846779099</v>
       </c>
       <c r="AL4">
-        <v>9.80392722719521</v>
+        <v>1.4743270691049299</v>
       </c>
       <c r="AM4">
-        <v>5.5879571711611504</v>
+        <v>0.73911912194185703</v>
       </c>
       <c r="AN4">
-        <v>2.91497899879203</v>
+        <v>0.36939569029276598</v>
       </c>
       <c r="AO4">
-        <v>1.4744596021085701</v>
+        <v>0.183888385719401</v>
       </c>
       <c r="AP4">
-        <v>0.73939429182498895</v>
+        <v>13.582810219631501</v>
       </c>
       <c r="AQ4">
-        <v>0.36995253843098302</v>
-      </c>
-    </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
+        <v>9.8037684449884193</v>
+      </c>
+      <c r="AR4">
+        <v>5.5879534085245197</v>
+      </c>
+      <c r="AS4">
+        <v>2.9149789183638299</v>
+      </c>
+      <c r="AT4">
+        <v>1.4744596814423501</v>
+      </c>
+      <c r="AU4">
+        <v>0.73939428633544502</v>
+      </c>
+      <c r="AV4">
+        <v>0.36995254170139003</v>
+      </c>
+      <c r="AW4">
+        <v>0.184996159801573</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>12.0232178519868</v>
+        <v>12.3236333991593</v>
       </c>
       <c r="C5">
-        <v>7.5845603223789899</v>
+        <v>7.5844094449156403</v>
       </c>
       <c r="D5">
-        <v>3.8389345637463199</v>
+        <v>3.8389216411457299</v>
       </c>
       <c r="E5">
-        <v>1.8961462184694799</v>
+        <v>1.8961455641767999</v>
       </c>
       <c r="F5">
-        <v>0.94334189818511005</v>
+        <v>0.94334187508559297</v>
       </c>
       <c r="G5">
-        <v>0.47100895251158897</v>
+        <v>0.47100895177966901</v>
       </c>
       <c r="H5">
-        <v>0.23541932435812901</v>
+        <v>0.23541932434198401</v>
       </c>
       <c r="I5">
-        <v>1.6138978998603499</v>
+        <v>0.117698939198842</v>
       </c>
       <c r="J5">
-        <v>1.0236140428617899</v>
+        <v>1.61692412818633</v>
       </c>
       <c r="K5">
-        <v>0.43858174106627201</v>
+        <v>1.02386975660121</v>
       </c>
       <c r="L5">
-        <v>0.19768502397383</v>
+        <v>0.438594707378758</v>
       </c>
       <c r="M5">
-        <v>9.5389231341616407E-2</v>
+        <v>0.19768547556730201</v>
       </c>
       <c r="N5">
-        <v>4.7234274742054903E-2</v>
+        <v>9.5389245827067204E-2</v>
       </c>
       <c r="O5">
-        <v>2.3558652045100801E-2</v>
+        <v>4.7234275197061998E-2</v>
       </c>
       <c r="P5">
-        <v>1.17919951857098</v>
+        <v>2.3558652065398599E-2</v>
       </c>
       <c r="Q5">
-        <v>0.728730551766683</v>
+        <v>1.17719853354898E-2</v>
       </c>
       <c r="R5">
-        <v>0.23824626379132399</v>
+        <v>1.1483741327805499</v>
       </c>
       <c r="S5">
-        <v>6.56411093847446E-2</v>
+        <v>0.72905334926009702</v>
       </c>
       <c r="T5">
-        <v>1.8201202282422599E-2</v>
+        <v>0.23827092628273699</v>
       </c>
       <c r="U5">
-        <v>6.0619647903313797E-3</v>
+        <v>6.5642649909128797E-2</v>
       </c>
       <c r="V5">
-        <v>2.5370345171348602E-3</v>
+        <v>1.8201290769398401E-2</v>
       </c>
       <c r="W5">
-        <v>1.1743341660893301</v>
+        <v>6.0619689962308296E-3</v>
       </c>
       <c r="X5">
-        <v>0.72572437213765195</v>
+        <v>2.5370347361262698E-3</v>
       </c>
       <c r="Y5">
-        <v>0.23704519450561501</v>
+        <v>1.2003777675154701E-3</v>
       </c>
       <c r="Z5">
-        <v>6.4765546273350599E-2</v>
+        <v>1.1430095511757199</v>
       </c>
       <c r="AA5">
-        <v>1.6654336481857199E-2</v>
+        <v>0.72604735611156801</v>
       </c>
       <c r="AB5">
-        <v>4.2024548513474903E-3</v>
+        <v>0.23706987730864201</v>
       </c>
       <c r="AC5">
-        <v>1.0574883118785201E-3</v>
+        <v>6.4767103161029502E-2</v>
       </c>
       <c r="AD5">
-        <v>1.1742854503802</v>
+        <v>1.6654433145747102E-2</v>
       </c>
       <c r="AE5">
-        <v>0.72569442649416505</v>
+        <v>4.2024608581355096E-3</v>
       </c>
       <c r="AF5">
-        <v>0.237035160902</v>
+        <v>1.05748893333109E-3</v>
       </c>
       <c r="AG5">
-        <v>6.4765337419273997E-2</v>
+        <v>2.7609386749146998E-4</v>
       </c>
       <c r="AH5">
-        <v>1.6657206785111699E-2</v>
+        <v>1.14295581739036</v>
       </c>
       <c r="AI5">
-        <v>4.2048268232490601E-3</v>
+        <v>0.72601741205552806</v>
       </c>
       <c r="AJ5">
-        <v>1.0550405989369299E-3</v>
+        <v>0.23705984357136001</v>
       </c>
       <c r="AK5">
-        <v>1.1742849632168799</v>
+        <v>6.4766894236630707E-2</v>
       </c>
       <c r="AL5">
-        <v>0.72569412704983705</v>
+        <v>1.6657304283531599E-2</v>
       </c>
       <c r="AM5">
-        <v>0.237035060788855</v>
+        <v>4.20483279939319E-3</v>
       </c>
       <c r="AN5">
-        <v>6.4765336627297596E-2</v>
+        <v>1.0550411609922901E-3</v>
       </c>
       <c r="AO5">
-        <v>1.66572412495616E-2</v>
+        <v>2.64130315141235E-4</v>
       </c>
       <c r="AP5">
-        <v>4.2048731847081902E-3</v>
+        <v>1.14295528004369</v>
       </c>
       <c r="AQ5">
-        <v>1.055090647767E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0.72601711262704705</v>
+      </c>
+      <c r="AR5">
+        <v>0.23705974345684</v>
+      </c>
+      <c r="AS5">
+        <v>6.4766893443914994E-2</v>
+      </c>
+      <c r="AT5">
+        <v>1.6657338745987401E-2</v>
+      </c>
+      <c r="AU5">
+        <v>4.20487916064031E-3</v>
+      </c>
+      <c r="AV5">
+        <v>1.05509121010227E-3</v>
+      </c>
+      <c r="AW5">
+        <v>2.6417915604450801E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:49" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -1123,8 +1220,9 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:49" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="8" t="s">
         <v>5</v>
@@ -1147,383 +1245,434 @@
       <c r="H7" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="I7" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1</v>
       </c>
       <c r="B8" s="3">
-        <f>B5</f>
-        <v>12.0232178519868</v>
+        <f t="shared" ref="B8:H8" si="0">B5</f>
+        <v>12.3236333991593</v>
       </c>
       <c r="C8" s="3">
-        <f>C5</f>
-        <v>7.5845603223789899</v>
+        <f t="shared" si="0"/>
+        <v>7.5844094449156403</v>
       </c>
       <c r="D8" s="3">
-        <f>D5</f>
-        <v>3.8389345637463199</v>
+        <f t="shared" si="0"/>
+        <v>3.8389216411457299</v>
       </c>
       <c r="E8" s="3">
-        <f>E5</f>
-        <v>1.8961462184694799</v>
+        <f t="shared" si="0"/>
+        <v>1.8961455641767999</v>
       </c>
       <c r="F8" s="3">
-        <f>F5</f>
-        <v>0.94334189818511005</v>
+        <f t="shared" si="0"/>
+        <v>0.94334187508559297</v>
       </c>
       <c r="G8" s="3">
-        <f>G5</f>
-        <v>0.47100895251158897</v>
+        <f t="shared" si="0"/>
+        <v>0.47100895177966901</v>
       </c>
       <c r="H8" s="3">
-        <f>H5</f>
-        <v>0.23541932435812901</v>
-      </c>
-    </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>0.23541932434198401</v>
+      </c>
+      <c r="I8" s="11">
+        <f>I5</f>
+        <v>0.117698939198842</v>
+      </c>
+    </row>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="5">
         <f>LOG(B8/C8, 2)</f>
-        <v>0.66468561073223675</v>
+        <v>0.70031891568947979</v>
       </c>
       <c r="D9" s="5">
-        <f t="shared" ref="D9:H9" si="0">LOG(C8/D8, 2)</f>
-        <v>0.98235958068852436</v>
+        <f t="shared" ref="D9:I9" si="1">LOG(C8/D8, 2)</f>
+        <v>0.98233573768852078</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="0"/>
-        <v>1.0176357492624659</v>
+        <f t="shared" si="1"/>
+        <v>1.0176313906849923</v>
       </c>
       <c r="F9" s="5">
-        <f t="shared" si="0"/>
-        <v>1.0072175687813187</v>
+        <f t="shared" si="1"/>
+        <v>1.0072171062855679</v>
       </c>
       <c r="G9" s="5">
-        <f t="shared" si="0"/>
-        <v>1.002026264355095</v>
+        <f t="shared" si="1"/>
+        <v>1.0020262312698307</v>
       </c>
       <c r="H9" s="5">
-        <f t="shared" si="0"/>
-        <v>1.0005217329073748</v>
-      </c>
-    </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>1.0005217307644518</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="1"/>
+        <v>1.0001314308709632</v>
+      </c>
+    </row>
+    <row r="10" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="6">
-        <f>I5</f>
-        <v>1.6138978998603499</v>
+        <f>J5</f>
+        <v>1.61692412818633</v>
       </c>
       <c r="C10" s="6">
-        <f>J5</f>
-        <v>1.0236140428617899</v>
+        <f t="shared" ref="C10:I10" si="2">K5</f>
+        <v>1.02386975660121</v>
       </c>
       <c r="D10" s="6">
-        <f>K5</f>
-        <v>0.43858174106627201</v>
+        <f t="shared" si="2"/>
+        <v>0.438594707378758</v>
       </c>
       <c r="E10" s="6">
-        <f>L5</f>
-        <v>0.19768502397383</v>
+        <f t="shared" si="2"/>
+        <v>0.19768547556730201</v>
       </c>
       <c r="F10" s="6">
-        <f>M5</f>
-        <v>9.5389231341616407E-2</v>
+        <f t="shared" si="2"/>
+        <v>9.5389245827067204E-2</v>
       </c>
       <c r="G10" s="6">
-        <f>N5</f>
-        <v>4.7234274742054903E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.7234275197061998E-2</v>
       </c>
       <c r="H10" s="6">
-        <f>O5</f>
-        <v>2.3558652045100801E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>2.3558652065398599E-2</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="2"/>
+        <v>1.17719853354898E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="5">
         <f>LOG(B10/C10, 2)</f>
-        <v>0.65687746736264507</v>
+        <v>0.65921977792940611</v>
       </c>
       <c r="D11" s="5">
-        <f t="shared" ref="D11:H11" si="1">LOG(C10/D10, 2)</f>
-        <v>1.2227541883914395</v>
+        <f t="shared" ref="D11:I11" si="3">LOG(C10/D10, 2)</f>
+        <v>1.223071898200532</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" si="1"/>
-        <v>1.1496421703696451</v>
+        <f t="shared" si="3"/>
+        <v>1.1496815261427955</v>
       </c>
       <c r="F11" s="5">
-        <f t="shared" si="1"/>
-        <v>1.0513052687943363</v>
+        <f t="shared" si="3"/>
+        <v>1.0513083454140435</v>
       </c>
       <c r="G11" s="5">
-        <f t="shared" si="1"/>
-        <v>1.0139923005127034</v>
+        <f t="shared" si="3"/>
+        <v>1.0139925056974823</v>
       </c>
       <c r="H11" s="5">
-        <f t="shared" si="1"/>
-        <v>1.0035771116477559</v>
-      </c>
-    </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>1.0035771243022109</v>
+      </c>
+      <c r="I11" s="5">
+        <f t="shared" si="3"/>
+        <v>1.0008993459122679</v>
+      </c>
+    </row>
+    <row r="12" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="6">
-        <f>P5</f>
-        <v>1.17919951857098</v>
+        <f>R5</f>
+        <v>1.1483741327805499</v>
       </c>
       <c r="C12" s="6">
-        <f>Q5</f>
-        <v>0.728730551766683</v>
+        <f t="shared" ref="C12:I12" si="4">S5</f>
+        <v>0.72905334926009702</v>
       </c>
       <c r="D12" s="6">
-        <f>R5</f>
-        <v>0.23824626379132399</v>
+        <f t="shared" si="4"/>
+        <v>0.23827092628273699</v>
       </c>
       <c r="E12" s="6">
-        <f>S5</f>
-        <v>6.56411093847446E-2</v>
+        <f t="shared" si="4"/>
+        <v>6.5642649909128797E-2</v>
       </c>
       <c r="F12" s="6">
-        <f>T5</f>
-        <v>1.8201202282422599E-2</v>
+        <f t="shared" si="4"/>
+        <v>1.8201290769398401E-2</v>
       </c>
       <c r="G12" s="6">
-        <f>U5</f>
-        <v>6.0619647903313797E-3</v>
+        <f t="shared" si="4"/>
+        <v>6.0619689962308296E-3</v>
       </c>
       <c r="H12" s="6">
-        <f>V5</f>
-        <v>2.5370345171348602E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>2.5370347361262698E-3</v>
+      </c>
+      <c r="I12" s="6">
+        <f t="shared" si="4"/>
+        <v>1.2003777675154701E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="5">
         <f>LOG(B12/C12, 2)</f>
-        <v>0.69435045899302761</v>
+        <v>0.65549644491891479</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" ref="D13:H13" si="2">LOG(C12/D12, 2)</f>
-        <v>1.6129318866516829</v>
+        <f t="shared" ref="D13:H13" si="5">LOG(C12/D12, 2)</f>
+        <v>1.6134214639397348</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="2"/>
-        <v>1.8597820629673363</v>
+        <f t="shared" si="5"/>
+        <v>1.8598975403526929</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" si="2"/>
-        <v>1.8505658707512349</v>
+        <f t="shared" si="5"/>
+        <v>1.8505927150241119</v>
       </c>
       <c r="G13" s="5">
-        <f t="shared" si="2"/>
-        <v>1.5861763732879866</v>
+        <f t="shared" si="5"/>
+        <v>1.5861823861107618</v>
       </c>
       <c r="H13" s="5">
-        <f t="shared" si="2"/>
-        <v>1.2566423247057372</v>
-      </c>
-    </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>1.2566432011426245</v>
+      </c>
+      <c r="I13" s="5">
+        <f>LOG(H12/I12, 2)</f>
+        <v>1.0796547685800413</v>
+      </c>
+    </row>
+    <row r="14" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="6">
-        <f>W5</f>
-        <v>1.1743341660893301</v>
+        <f>Z5</f>
+        <v>1.1430095511757199</v>
       </c>
       <c r="C14" s="6">
-        <f>X5</f>
-        <v>0.72572437213765195</v>
+        <f t="shared" ref="C14:I14" si="6">AA5</f>
+        <v>0.72604735611156801</v>
       </c>
       <c r="D14" s="6">
-        <f>Y5</f>
-        <v>0.23704519450561501</v>
+        <f t="shared" si="6"/>
+        <v>0.23706987730864201</v>
       </c>
       <c r="E14" s="6">
-        <f>Z5</f>
-        <v>6.4765546273350599E-2</v>
+        <f t="shared" si="6"/>
+        <v>6.4767103161029502E-2</v>
       </c>
       <c r="F14" s="6">
-        <f>AA5</f>
-        <v>1.6654336481857199E-2</v>
+        <f t="shared" si="6"/>
+        <v>1.6654433145747102E-2</v>
       </c>
       <c r="G14" s="6">
-        <f>AB5</f>
-        <v>4.2024548513474903E-3</v>
+        <f t="shared" si="6"/>
+        <v>4.2024608581355096E-3</v>
       </c>
       <c r="H14" s="6">
-        <f>AC5</f>
-        <v>1.0574883118785201E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>1.05748893333109E-3</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="6"/>
+        <v>2.7609386749146998E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="5">
         <f>LOG(B14/C14, 2)</f>
-        <v>0.69434937090767113</v>
+        <v>0.65470190346330637</v>
       </c>
       <c r="D15" s="5">
-        <f t="shared" ref="D15:H15" si="3">LOG(C14/D14, 2)</f>
-        <v>1.6142595747987734</v>
+        <f t="shared" ref="D15:I15" si="7">LOG(C14/D14, 2)</f>
+        <v>1.614751288397827</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="3"/>
-        <v>1.8718637034301588</v>
+        <f t="shared" si="7"/>
+        <v>1.8719792388264429</v>
       </c>
       <c r="F15" s="5">
-        <f t="shared" si="3"/>
-        <v>1.9593286604345856</v>
+        <f t="shared" si="7"/>
+        <v>1.9593549671509451</v>
       </c>
       <c r="G15" s="5">
-        <f t="shared" si="3"/>
-        <v>1.986593652166698</v>
+        <f t="shared" si="7"/>
+        <v>1.9865999636103113</v>
       </c>
       <c r="H15" s="5">
-        <f t="shared" si="3"/>
-        <v>1.9905906023651054</v>
-      </c>
-    </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>1.9905918166567573</v>
+      </c>
+      <c r="I15" s="5">
+        <f t="shared" si="7"/>
+        <v>1.9374118168417385</v>
+      </c>
+    </row>
+    <row r="16" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="6">
-        <f>AD5</f>
-        <v>1.1742854503802</v>
+        <f>AH5</f>
+        <v>1.14295581739036</v>
       </c>
       <c r="C16" s="6">
-        <f>AE5</f>
-        <v>0.72569442649416505</v>
+        <f t="shared" ref="C16:I16" si="8">AI5</f>
+        <v>0.72601741205552806</v>
       </c>
       <c r="D16" s="6">
-        <f>AF5</f>
-        <v>0.237035160902</v>
+        <f t="shared" si="8"/>
+        <v>0.23705984357136001</v>
       </c>
       <c r="E16" s="6">
-        <f>AG5</f>
-        <v>6.4765337419273997E-2</v>
+        <f t="shared" si="8"/>
+        <v>6.4766894236630707E-2</v>
       </c>
       <c r="F16" s="6">
-        <f>AH5</f>
-        <v>1.6657206785111699E-2</v>
+        <f t="shared" si="8"/>
+        <v>1.6657304283531599E-2</v>
       </c>
       <c r="G16" s="6">
-        <f>AI5</f>
-        <v>4.2048268232490601E-3</v>
+        <f t="shared" si="8"/>
+        <v>4.20483279939319E-3</v>
       </c>
       <c r="H16" s="6">
-        <f>AJ5</f>
-        <v>1.0550405989369299E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>1.0550411609922901E-3</v>
+      </c>
+      <c r="I16" s="6">
+        <f t="shared" si="8"/>
+        <v>2.64130315141235E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="5">
         <f>LOG(B16/C16, 2)</f>
-        <v>0.69434905266922531</v>
+        <v>0.65469358130372168</v>
       </c>
       <c r="D17" s="5">
-        <f t="shared" ref="D17:H17" si="4">LOG(C16/D16, 2)</f>
-        <v>1.6142611109005269</v>
+        <f t="shared" ref="D17:H17" si="9">LOG(C16/D16, 2)</f>
+        <v>1.6147528485924807</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="4"/>
-        <v>1.8718072883873149</v>
+        <f t="shared" si="9"/>
+        <v>1.8719228307829743</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="4"/>
-        <v>1.9590753872046494</v>
+        <f t="shared" si="9"/>
+        <v>1.9591016216303565</v>
       </c>
       <c r="G17" s="5">
-        <f t="shared" si="4"/>
-        <v>1.9860282091427306</v>
+        <f t="shared" si="9"/>
+        <v>1.9860346030996865</v>
       </c>
       <c r="H17" s="5">
-        <f t="shared" si="4"/>
-        <v>1.9947478677412915</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <f t="shared" si="9"/>
+        <v>1.994749149610207</v>
+      </c>
+      <c r="I17" s="5">
+        <f>LOG(H16/I16, 2)</f>
+        <v>1.9979774856367944</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="6">
-        <f>AK5</f>
-        <v>1.1742849632168799</v>
+        <f>AP5</f>
+        <v>1.14295528004369</v>
       </c>
       <c r="C18" s="6">
-        <f>AL5</f>
-        <v>0.72569412704983705</v>
+        <f t="shared" ref="C18:I18" si="10">AQ5</f>
+        <v>0.72601711262704705</v>
       </c>
       <c r="D18" s="6">
-        <f>AM5</f>
-        <v>0.237035060788855</v>
+        <f t="shared" si="10"/>
+        <v>0.23705974345684</v>
       </c>
       <c r="E18" s="6">
-        <f>AN5</f>
-        <v>6.4765336627297596E-2</v>
+        <f t="shared" si="10"/>
+        <v>6.4766893443914994E-2</v>
       </c>
       <c r="F18" s="6">
-        <f>AO5</f>
-        <v>1.66572412495616E-2</v>
+        <f t="shared" si="10"/>
+        <v>1.6657338745987401E-2</v>
       </c>
       <c r="G18" s="6">
-        <f>AP5</f>
-        <v>4.2048731847081902E-3</v>
+        <f t="shared" si="10"/>
+        <v>4.20487916064031E-3</v>
       </c>
       <c r="H18" s="6">
-        <f>AQ5</f>
-        <v>1.055090647767E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <f t="shared" si="10"/>
+        <v>1.05509121010227E-3</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" si="10"/>
+        <v>2.6417915604450801E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8"/>
       <c r="B19" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="10">
         <f>LOG(B18/C18, 2)</f>
-        <v>0.69434904945498666</v>
+        <v>0.65469349804328481</v>
       </c>
       <c r="D19" s="10">
-        <f t="shared" ref="D19:H19" si="5">LOG(C18/D18, 2)</f>
-        <v>1.6142611249296523</v>
+        <f t="shared" ref="D19:I19" si="11">LOG(C18/D18, 2)</f>
+        <v>1.6147528628628542</v>
       </c>
       <c r="E19" s="10">
-        <f t="shared" si="5"/>
-        <v>1.8718066966986018</v>
+        <f t="shared" si="11"/>
+        <v>1.8719222391653809</v>
       </c>
       <c r="F19" s="10">
-        <f t="shared" si="5"/>
-        <v>1.9590723845701661</v>
+        <f t="shared" si="11"/>
+        <v>1.9590986191700104</v>
       </c>
       <c r="G19" s="10">
-        <f t="shared" si="5"/>
-        <v>1.986015287397402</v>
+        <f t="shared" si="11"/>
+        <v>1.9860216812595251</v>
       </c>
       <c r="H19" s="10">
-        <f t="shared" si="5"/>
-        <v>1.9946953377892869</v>
+        <f t="shared" si="11"/>
+        <v>1.9946966192165729</v>
+      </c>
+      <c r="I19" s="10">
+        <f t="shared" si="11"/>
+        <v>1.9977791754993166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>